<commit_message>
messaging - sync messaging service
</commit_message>
<xml_diff>
--- a/documents/vm/vmWareOnboarding.xlsx
+++ b/documents/vm/vmWareOnboarding.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web\image-ai\ai-web-micro-services\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web\image-ai\ai-web-micro-services\documents\vm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7603C0-821A-4409-9A87-D5CC9BEEB9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586571F8-16E8-4C0D-AA54-6B94C8BB60D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vmware" sheetId="1" r:id="rId1"/>
@@ -2262,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6D97B2-BF14-4519-A72E-56FD81FC020C}">
   <dimension ref="A2:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2835,8 +2835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C6DC3E-0207-4183-A84C-6F570A0F88D6}">
   <dimension ref="A2:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>